<commit_message>
option 3& fix MLP error
</commit_message>
<xml_diff>
--- a/data/performance_sheets_option3/window3/BA47 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets_option3/window3/BA47 Overall Model Peformance Results.xlsx
@@ -770,19 +770,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.04691346051182275</v>
+        <v>0.04691346051182278</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1865129431110522</v>
+        <v>0.1865129431110523</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2643682770640483</v>
+        <v>0.2643682770640485</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2165951534818421</v>
+        <v>0.2165951534818422</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>31.91825104663494</v>
+        <v>31.91825104663497</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -800,19 +800,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.02885241618130124</v>
+        <v>0.0288524161813012</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1334341014862883</v>
+        <v>0.1334341014862882</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1803507468632586</v>
+        <v>0.1803507468632584</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1698599899367159</v>
+        <v>0.1698599899367158</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>20.41689859926331</v>
+        <v>20.41689859926328</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -950,10 +950,10 @@
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>0.01895305492072721</v>
+        <v>0.0189530549207272</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.09227082658041728</v>
+        <v>0.09227082658041726</v>
       </c>
       <c r="N10" s="8" t="n">
         <v>0.1135212951227853</v>
@@ -1338,19 +1338,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.01890510719856978</v>
+        <v>0.01939718884886394</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.1168679506352037</v>
+        <v>0.1197960101877554</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.1556125386578255</v>
+        <v>0.1616682021066557</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.137495844295636</v>
+        <v>0.1392737909617741</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>17.24925646147195</v>
+        <v>17.9508482224712</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -1368,19 +1368,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.01792337070693652</v>
+        <v>0.01844870504145972</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>0.1105820600460787</v>
+        <v>0.1119564287566911</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.1459123134321283</v>
+        <v>0.1470179569967989</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>0.1338781935452392</v>
+        <v>0.1358260101801556</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>16.16027842127829</v>
+        <v>16.29765059531649</v>
       </c>
     </row>
     <row r="18" ht="56.1" customHeight="1">
@@ -1621,25 +1621,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.0217911321669817</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1227282732725143</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1767432391643524</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.1476181972758836</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>17.44444966316223</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.02165912091732025</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1256087422370911</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.1817547380924225</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.147170380570685</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>17.86060035228729</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -1647,25 +1683,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.01469117496162653</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.09587417542934418</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.120208814740181</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1212071572211251</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>12.64975219964981</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.01295225042849779</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.09289656579494476</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.1197231560945511</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1138079541530283</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>12.30364441871643</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -1905,19 +1977,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>2.151490204373055e-08</v>
+        <v>2.151490204321804e-08</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0001149290634037882</v>
+        <v>0.0001149290634032826</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>4.496607283100686e-05</v>
+        <v>4.49660728309747e-05</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.0001466795897312593</v>
+        <v>0.0001466795897295122</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.004496634602319426</v>
+        <v>0.004496634602316195</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -1935,19 +2007,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>1.548598766413142e-08</v>
+        <v>1.54859876634327e-08</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>9.622400242550361e-05</v>
+        <v>9.622400243376651e-05</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>3.910750176585254e-05</v>
+        <v>3.910750176858316e-05</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.0001244427083606405</v>
+        <v>0.0001244427083578331</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.003910714390190721</v>
+        <v>0.003910714390463805</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -2535,19 +2607,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.7799251586075057</v>
+        <v>0.7803068611611964</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.7510675446688764</v>
+        <v>0.7512715230520056</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.2919199500228065</v>
+        <v>0.2919954481813</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.8831337150214036</v>
+        <v>0.8833497954724371</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>33.92636636788297</v>
+        <v>33.93730258588248</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -2565,19 +2637,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.8594860923695925</v>
+        <v>0.8612561323074759</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.7808953612654808</v>
+        <v>0.7817629233959406</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.3041204447632288</v>
+        <v>0.3046076294441339</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.9270847277188814</v>
+        <v>0.9280388635760228</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>35.24719331879736</v>
+        <v>35.2859249278901</v>
       </c>
     </row>
     <row r="19" ht="27.95" customHeight="1">
@@ -2756,25 +2828,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.2674514949321747</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.380928635597229</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1806354075670242</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.5171571278945836</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>15.05910754203796</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.05}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.1869288980960846</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.3010452389717102</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.1475583761930466</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.4323527472979495</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>12.16488480567932</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -2782,25 +2890,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.1012623086571693</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.2823186814785004</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1045922711491585</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.3182173921349513</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>10.33300086855888</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.109317310154438</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.2756785154342651</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.09670362621545792</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.3306316835308407</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>10.21770462393761</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -3037,19 +3181,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>2.515470481349775e-08</v>
+        <v>2.515470481186856e-08</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0001085290845384916</v>
+        <v>0.0001085290845360099</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>3.827987958425994e-05</v>
+        <v>3.827987958348157e-05</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.0001586023480705685</v>
+        <v>0.0001586023480654324</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.003828115025746689</v>
+        <v>0.00382811502566884</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -3067,19 +3211,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>2.482851003973285e-08</v>
+        <v>2.482851004198971e-08</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.0001064385411046639</v>
+        <v>0.0001064385411138787</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>3.745256903121443e-05</v>
+        <v>3.745256903489967e-05</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.0001575706509465924</v>
+        <v>0.0001575706509537538</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.003745373181212203</v>
+        <v>0.003745373181580746</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -3187,7 +3331,7 @@
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0.1650576266140641</v>
+        <v>0.165057626614064</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>0.3657245281525631</v>
@@ -3196,7 +3340,7 @@
         <v>0.1365044190327726</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.406272847497915</v>
+        <v>0.4062728474979149</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>14.03656891048017</v>
@@ -3667,19 +3811,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.4977871370044834</v>
+        <v>0.4961515940573445</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.6365204936198424</v>
+        <v>0.6355707297994377</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.230193064746858</v>
+        <v>0.2298642102740325</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.705540315647861</v>
+        <v>0.7043802907927965</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>26.78763024431703</v>
+        <v>26.74103597680372</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -3697,19 +3841,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.8998347682852245</v>
+        <v>0.8999307094483407</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.8126481568559896</v>
+        <v>0.8126233505749105</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.2984097121096361</v>
+        <v>0.2983900205689163</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.9485962092930924</v>
+        <v>0.9486467780203234</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>36.93014004863068</v>
+        <v>36.92879985294301</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -3888,25 +4032,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.1026597693562508</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2710290551185608</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1064721792936325</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.3204056325289097</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>10.20876318216324</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.1163084954023361</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2423282265663147</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.09643658250570297</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.3410403134562484</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>9.165143966674805</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -3914,25 +4094,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.124664418399334</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.2624711692333221</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.08989758789539337</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.353078487590697</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>9.652020782232285</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.03432462736964226</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.1458222419023514</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.05479502305388451</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1852690674927746</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>5.249214917421341</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -4169,19 +4385,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>7.021215941041383e-07</v>
+        <v>7.021215941080112e-07</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0007023216807058892</v>
+        <v>0.0007023216807098393</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.0002582451862565843</v>
+        <v>0.0002582451862575858</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.0008379269622730482</v>
+        <v>0.0008379269622753591</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.0258291356673881</v>
+        <v>0.02582913566748826</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -4199,19 +4415,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>6.554230804584974e-07</v>
+        <v>6.554230804551622e-07</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.0006687757049760148</v>
+        <v>0.0006687757049799648</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.000248280014130404</v>
+        <v>0.0002482800141315288</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.0008095820405977997</v>
+        <v>0.0008095820405957399</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.02483249892036948</v>
+        <v>0.02483249892048195</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -4829,19 +5045,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.9307541728442571</v>
+        <v>0.9224328285634108</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.9286336952438493</v>
+        <v>0.9248283894822722</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.3312287109954221</v>
+        <v>0.3298674116128356</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.964756017262529</v>
+        <v>0.9604336669252129</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>40.28372900819173</v>
+        <v>40.06862747429311</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -5020,25 +5236,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.04965189844369888</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1859682500362396</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.06674764305353165</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2228270594961458</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>6.734443455934525</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.04843815788626671</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1703043282032013</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.06120994687080383</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2200867053828257</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>6.157742813229561</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -5046,25 +5298,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.04839068651199341</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.190775528550148</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.06542883813381195</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2199788319634264</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>6.787993013858795</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.09384477138519287</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.2683385610580444</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.09375232458114624</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.3063409397798356</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>9.975908696651459</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -5329,10 +5617,10 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.06106904735098521</v>
+        <v>0.0610690473509852</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.156049111848684</v>
+        <v>0.1560491118486841</v>
       </c>
       <c r="N7" s="8" t="n">
         <v>1.365485768840762</v>
@@ -5341,7 +5629,7 @@
         <v>0.2471215234474432</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>30.12491575558444</v>
+        <v>30.12491575558445</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -5458,7 +5746,7 @@
         <v>1.55614290264398</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.2871854419846916</v>
+        <v>0.2871854419846915</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>31.27954035619874</v>
@@ -5929,19 +6217,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.07333538539684481</v>
+        <v>0.07329802751971846</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.1859186800320309</v>
+        <v>0.1858589856471209</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>1.457503169300415</v>
+        <v>1.457293716966848</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2708050690013848</v>
+        <v>0.2707360846280349</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>34.22608490856766</v>
+        <v>34.21951316829636</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -5959,19 +6247,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.06803120156894521</v>
+        <v>0.06813670750814504</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.181896822445905</v>
+        <v>0.1822789669474415</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>1.402084571572941</v>
+        <v>1.403109030600282</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2608279156243541</v>
+        <v>0.2610300892773572</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>33.93177008148221</v>
+        <v>33.98478157891402</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -6150,25 +6438,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.05867500230669975</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1619278639554977</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>1.319299936294556</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2422292350371849</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>33.28613936901093</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.06110038608312607</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1441348642110825</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>1.354312539100647</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2471849228475031</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>27.69750654697418</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -6176,25 +6500,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 20, 'lr': 0.01, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.1497609615325928</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.3181955516338348</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.5217246413230896</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.3869896142438357</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>68.71525645256042</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.05824960023164749</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.186415508389473</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.6479576230049133</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.2413495395306307</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>33.00651907920837</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -6429,13 +6789,13 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.05118941941207773</v>
+        <v>0.05118941941207775</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>0.1273370174838717</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.321598690600178</v>
+        <v>1.321598690600179</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0.226250788754598</v>
@@ -6459,19 +6819,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.05123666249868918</v>
+        <v>0.05123666249868927</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1288673666514995</v>
+        <v>0.1288673666514994</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>1.320984477050704</v>
+        <v>1.320984477050705</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2263551689241692</v>
+        <v>0.2263551689241694</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>25.61218087449125</v>
+        <v>25.61218087449124</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -6997,19 +7357,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.05775681340367533</v>
+        <v>0.05700208640125029</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.1426073323123181</v>
+        <v>0.1420664932461579</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>1.396626183310386</v>
+        <v>1.389657232677677</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.2403264725403245</v>
+        <v>0.2387510971728723</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>27.5939829036763</v>
+        <v>27.54113702852483</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -7027,19 +7387,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.0602488347433603</v>
+        <v>0.06044988857564605</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>0.1433945144302864</v>
+        <v>0.1423371959308086</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>1.420263513693134</v>
+        <v>1.428384492631226</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>0.2454563805309617</v>
+        <v>0.2458655904669176</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>27.18587284403875</v>
+        <v>27.02862308978686</v>
       </c>
     </row>
     <row r="18" ht="42" customHeight="1">
@@ -7059,19 +7419,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.05692905620279216</v>
+        <v>0.05692833917967938</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.1492537951212967</v>
+        <v>0.1492084773436706</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>1.377143932734083</v>
+        <v>1.377287294256909</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2385981060335395</v>
+        <v>0.238596603453778</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>29.17832625916635</v>
+        <v>29.17623343413727</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -7089,19 +7449,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.05719159780466332</v>
+        <v>0.05716062069912854</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.1483664565535739</v>
+        <v>0.1483322388350397</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>1.38162594647659</v>
+        <v>1.381590555008128</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2391476485451264</v>
+        <v>0.2390828741234481</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>29.0927130997726</v>
+        <v>29.08704957171673</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -7280,25 +7640,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.05}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.1003178134560585</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2373921275138855</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>1.610312461853027</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.3167298745872553</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>40.98810851573944</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.05}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.08515667170286179</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2114171832799911</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>1.415354013442993</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2918161607979616</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>39.65379595756531</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -7306,25 +7702,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.0485677681863308</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1434234231710434</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.5662615895271301</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2203809614878989</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>26.50611400604248</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.05699502676725388</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.1296510249376297</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.6072970628738403</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.238736312209211</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>22.8194072842598</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -7559,7 +7991,7 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.04000674610406071</v>
+        <v>0.04000674610406073</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>0.1158203960128188</v>
@@ -7568,10 +8000,10 @@
         <v>1.22911721571609</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2000168645491192</v>
+        <v>0.2000168645491193</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>23.842678626271</v>
+        <v>23.84267862627098</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -7598,7 +8030,7 @@
         <v>1.218614462923644</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.1976729687480411</v>
+        <v>0.197672968748041</v>
       </c>
       <c r="P7" s="8" t="n">
         <v>23.39720696724434</v>
@@ -8410,25 +8842,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': Tanh(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.0588083304464817</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1911791414022446</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.7994844913482666</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2425042895424361</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>52.63201594352722</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.01}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.06715608388185501</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2117420732975006</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>1.071150183677673</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2591449090409746</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>49.70252513885498</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -8436,25 +8904,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.08311735093593597</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.2481769323348999</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.5903306603431702</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2883007994021799</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>44.23376321792603</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.03607242554426193</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.1095123961567879</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.4245294332504272</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1899274217806948</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>19.1850483417511</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -8695,7 +9199,7 @@
         <v>0.3290837317365065</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.5893408455031429</v>
+        <v>0.5893408455031428</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0.7463995213689421</v>
@@ -8722,10 +9226,10 @@
         <v>0.5836818109352441</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.312714877982272</v>
+        <v>0.3127148779822719</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.602695028936157</v>
+        <v>0.6026950289361571</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>0.7639907139064218</v>
@@ -9253,23 +9757,23 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'loss': 'linear', 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 200, 'loss': 'square', 'learning_rate': 0.01}</t>
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.6139783800767745</v>
+        <v>0.6170308977843502</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.370016466737731</v>
+        <v>0.370004655692372</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.6227233797552022</v>
+        <v>0.6236574649584318</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.7835677252648775</v>
+        <v>0.7855131429736553</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>17.80660610580415</v>
+        <v>17.79690777099726</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -9319,19 +9823,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.5792624463248209</v>
+        <v>0.5795268577459554</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.3704392503256365</v>
+        <v>0.3707785285260347</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.6076212468196508</v>
+        <v>0.6077818363068195</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.7610929288364339</v>
+        <v>0.7612666141017583</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>18.02390607629724</v>
+        <v>18.03598296209959</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -9349,19 +9853,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.5899101782335241</v>
+        <v>0.5898471796886336</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.3630879101928352</v>
+        <v>0.3629453006919038</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.608231639148119</v>
+        <v>0.6081738045534889</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.7680561035715582</v>
+        <v>0.7680150907948577</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>17.70650300362469</v>
+        <v>17.70114487090571</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -9540,25 +10044,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.6078977584838867</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.3940085470676422</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.5959764122962952</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.7796779838394097</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>18.82291585206985</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.666482150554657</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.4458754360675812</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.65900057554245</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.8163835805273505</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>20.59878706932068</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -9566,25 +10106,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.2549581527709961</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.3294937014579773</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.2158469408750534</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.5049338102870475</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>14.46121037006378</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.3008857071399689</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.4062292873859406</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.2318483293056488</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.5485304979123484</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>18.52411031723022</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -9819,19 +10395,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.51554079861922</v>
+        <v>0.5155407986192199</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.300601984587709</v>
+        <v>0.3006019845877088</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>0.5959316637386596</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.718011698107503</v>
+        <v>0.7180116981075029</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>15.26681300847412</v>
+        <v>15.26681300847411</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -9849,7 +10425,7 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.5723999367004201</v>
+        <v>0.57239993670042</v>
       </c>
       <c r="M7" s="8" t="n">
         <v>0.3089059745282263</v>
@@ -9858,7 +10434,7 @@
         <v>0.623098472661228</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.7565711709419148</v>
+        <v>0.7565711709419147</v>
       </c>
       <c r="P7" s="8" t="n">
         <v>15.64152761325156</v>
@@ -10670,25 +11246,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.6580232381820679</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.4510447978973389</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.6776918172836304</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.8111863153320992</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>20.870740711689</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.6281725168228149</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.459376722574234</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.650696873664856</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.7925733510677828</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>21.31986171007156</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -10696,25 +11308,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 10, 'lr': 0.1, 'batch_size': 32}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.2550119757652283</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.3618099987506866</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1926373094320297</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.5049871045534017</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>15.69518148899078</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.2490645349025726</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.3009190559387207</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.18534916639328</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.4990636581665436</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>13.21420222520828</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -10949,19 +11597,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.3874259376212881</v>
+        <v>0.3874259376212871</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.2777114738634545</v>
+        <v>0.277711473863455</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2593953539199084</v>
+        <v>0.2593953539199083</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.6224354887225568</v>
+        <v>0.6224354887225559</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>14.13148955516597</v>
+        <v>14.13148955516599</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -11102,7 +11750,7 @@
         <v>0.5209690494891716</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.3100119610220168</v>
+        <v>0.3100119610220169</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>0.2943555531777585</v>
@@ -11800,25 +12448,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.6284239292144775</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.3963180184364319</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.3396179676055908</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.7927319403269163</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>17.83523559570312</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.6248776912689209</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.4287548661231995</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.3558781147003174</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.7904920564236688</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>19.37090158462524</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -11826,25 +12510,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 10, 'lr': 0.1, 'batch_size': 32}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.2584697306156158</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.3128498494625092</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1795715689659119</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.5083991843184014</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>13.23589086532593</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.274994432926178</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.4160744845867157</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.2013571411371231</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.524399116061591</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>17.00493693351746</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -12079,19 +12799,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1386605782654944</v>
+        <v>0.1386605782654949</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3124623015815093</v>
+        <v>0.3124623015815098</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.4461094991200819</v>
+        <v>0.4461094991200826</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.3723715594208216</v>
+        <v>0.3723715594208222</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>45.2134898228861</v>
+        <v>45.21348982288622</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -12750,13 +13470,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.02739814110100269</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1404089778661728</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.2006563097238541</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.1655238384674627</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>20.07513493299484</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -12776,13 +13514,31 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.05128805339336395</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1691429764032364</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.2039474546909332</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2264686587441272</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>23.75997602939606</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
@@ -13011,19 +13767,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.03287235298010503</v>
+        <v>0.032872352980105</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1193170587321527</v>
+        <v>0.1193170587321526</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>0.1710301538722946</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.1813073439773057</v>
+        <v>0.1813073439773056</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>18.84215654103124</v>
+        <v>18.84215654103123</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -13047,13 +13803,13 @@
         <v>0.118477669977406</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1583014124449199</v>
+        <v>0.15830141244492</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>0.1800317217503902</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>17.60310688830728</v>
+        <v>17.60310688830729</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -13579,19 +14335,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.02478535353214623</v>
+        <v>0.02430025643710861</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.08881363282711609</v>
+        <v>0.08907931170583336</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.1158961239217796</v>
+        <v>0.116101998447642</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.1574336480303567</v>
+        <v>0.1558853952014383</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>13.5609405391185</v>
+        <v>13.56347612756473</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -13862,25 +14618,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.02430844306945801</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1175113841891289</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.3047723770141602</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.155911651487174</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>19.86031085252762</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.02577761560678482</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1187585666775703</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.2902319133281708</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.1605540893493057</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>19.86660063266754</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -13888,25 +14680,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.01415591593831778</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.09747026115655899</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1334710717201233</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1189786364786459</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>13.44578862190247</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.01728280633687973</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.1147612333297729</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.1751942485570908</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.131464087631869</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>16.57136082649231</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -14141,19 +14969,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.2467826283452061</v>
+        <v>0.2467826283452072</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.388514580633976</v>
+        <v>0.3885145806339769</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.6149863109339231</v>
+        <v>0.6149863109339252</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.4967722097150827</v>
+        <v>0.4967722097150838</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>74.62512569230738</v>
+        <v>74.62512569230748</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -14583,19 +15411,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.01407787692486633</v>
+        <v>0.01360011526008771</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.09690466002434857</v>
+        <v>0.09787147916631248</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.1494723804110198</v>
+        <v>0.1522244291730688</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.1186502293502475</v>
+        <v>0.1166195320694081</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>14.88708441571576</v>
+        <v>15.2215394040112</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -14812,13 +15640,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.04179665818810463</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1725544482469559</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.3131817579269409</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2044423101711205</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>25.92292428016663</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -14838,13 +15684,31 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.010647002607584</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.08922901749610901</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1295663863420486</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1031843137670838</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>12.86061704158783</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
@@ -15076,10 +15940,10 @@
         <v>1.524633521049607</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.9061769672805853</v>
+        <v>0.9061769672805854</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.322648818574931</v>
+        <v>1.32264881857493</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>1.234760511617377</v>
@@ -15190,7 +16054,7 @@
         <v>0.01945301441017687</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.09829239473499626</v>
+        <v>0.09829239473499631</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>0.2173411015291291</v>
@@ -15744,13 +16608,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.02604903653264046</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1106068193912506</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.3074289560317993</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.1613971391711776</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>18.96805018186569</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -15770,13 +16652,31 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.0114212641492486</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.08130958676338196</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1076293438673019</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1068703146306242</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>11.04032546281815</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
@@ -16005,19 +16905,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.086878532347093</v>
+        <v>1.086878532347104</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.7143386181492097</v>
+        <v>0.7143386181492122</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.2690915174269083</v>
+        <v>0.2690915174269093</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.04253466721596</v>
+        <v>1.042534667215966</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>30.1773677515132</v>
+        <v>30.17736775151324</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -16447,19 +17347,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.04011222805589833</v>
+        <v>0.03431248574281102</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.1631130873061411</v>
+        <v>0.1499330470573809</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.05887781600270805</v>
+        <v>0.05392017156273129</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.200280373616334</v>
+        <v>0.1852362970446425</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>5.98697666743605</v>
+        <v>5.430373685115762</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -16676,13 +17576,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.04552879929542542</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1795201897621155</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.06451156735420227</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2133747859880014</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>6.492049992084503</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -16702,13 +17620,31 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.0205940343439579</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1151023358106613</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.04053305089473724</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1435062170916574</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>4.052479937672615</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
@@ -16937,19 +17873,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>13.47039894701386</v>
+        <v>13.47039894701384</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>3.187357589496772</v>
+        <v>3.187357589496769</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.210081305327064</v>
+        <v>1.210081305327063</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>3.670204210532959</v>
+        <v>3.670204210532956</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>124.4510893863022</v>
+        <v>124.4510893863021</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -17379,19 +18315,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.1859451575328536</v>
+        <v>0.1426742672054963</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.3412306553795695</v>
+        <v>0.3055886697495041</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.123304426129212</v>
+        <v>0.1123618228782966</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.4312135869065973</v>
+        <v>0.3777224737892839</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>13.66457183207071</v>
+        <v>12.28345490248566</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -17608,13 +18544,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.05}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.09214998781681061</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2401342391967773</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.09445954114198685</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.3035621646661695</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>9.066081792116165</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -17634,13 +18588,31 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.05132895335555077</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1917637586593628</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.07115644216537476</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2265589401360069</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>6.928303092718124</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
@@ -17869,19 +18841,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>20.58693804808685</v>
+        <v>20.58693804808689</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>3.582806496431205</v>
+        <v>3.58280649643121</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.408202573752558</v>
+        <v>1.40820257375256</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>4.537283113063021</v>
+        <v>4.537283113063024</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>101.8058318287785</v>
+        <v>101.8058318287787</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -17986,10 +18958,10 @@
         <v>0.1372342812876428</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.1901703231418024</v>
+        <v>0.1901703231418023</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.08814177494580269</v>
+        <v>0.08814177494580273</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>0.3704514560474055</v>
@@ -18540,13 +19512,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.1870554387569427</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2859668135643005</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1426877528429031</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.4324990621457378</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>11.61508187651634</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -18566,13 +19556,31 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.06348109990358353</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.2124339193105698</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.07952271401882172</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2519545592038047</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>7.768917828798294</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
@@ -18804,16 +19812,16 @@
         <v>0.03318441325406175</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1252566644950564</v>
+        <v>0.1252566644950565</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1683210465241229</v>
+        <v>0.168321046524123</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>0.1821658948707517</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>18.32138605344866</v>
+        <v>18.32138605344867</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -18831,19 +19839,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.03796050833193026</v>
+        <v>0.03796050833193025</v>
       </c>
       <c r="M7" s="8" t="n">
         <v>0.1360457340208823</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1916771712754865</v>
+        <v>0.1916771712754864</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>0.1948345665736197</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>20.06547374668844</v>
+        <v>20.06547374668843</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -18993,7 +20001,7 @@
         <v>0.1515755739326487</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>15.56475665151888</v>
+        <v>15.56475665151889</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -19369,19 +20377,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0.01193295987297362</v>
+        <v>0.01152834384551033</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>0.08317032605991503</v>
+        <v>0.08049304027375079</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.1265825208336558</v>
+        <v>0.1223191334925994</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>0.1092380880140879</v>
+        <v>0.1073701254796246</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>13.74447472212602</v>
+        <v>13.17363842512736</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -19652,25 +20660,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.03183382004499435</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1451146006584167</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.2606112062931061</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.1784203464994796</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>22.14545011520386</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.03279947489500046</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1493251770734787</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.2670179307460785</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.1811062530532849</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>22.75210618972778</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -19678,25 +20722,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.01324021071195602</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1013761609792709</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.1543918699026108</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1150661145253285</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>14.4150048494339</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.00982936006039381</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.0869218185544014</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.1269160807132721</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.09914312916381957</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>12.27490678429604</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -19937,10 +21017,10 @@
         <v>0.3031012090569072</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1053925303944741</v>
+        <v>0.105392530394474</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.3998718376710122</v>
+        <v>0.3998718376710121</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>11.41564632551585</v>
@@ -19964,7 +21044,7 @@
         <v>0.3044080361402861</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.4577233799393352</v>
+        <v>0.4577233799393349</v>
       </c>
       <c r="N7" s="8" t="n">
         <v>0.1619838810195003</v>
@@ -20782,25 +21862,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.04837033152580261</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1806066334247589</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.06472466886043549</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2199325613132412</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>6.528839468955994</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.03832607343792915</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1580208390951157</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.05743037909269333</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.1957704610964819</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>5.714422091841698</v>
+      </c>
     </row>
     <row r="23" ht="57" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -20808,25 +21924,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.03988679125905037</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1598358005285263</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.05459548160433769</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1997167776103209</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>5.637476965785027</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.03358138352632523</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.1423494666814804</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.04841142892837524</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1832522401672766</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>5.000969022512436</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -21074,7 +22226,7 @@
         <v>0.5097608304627678</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>15.9381803972159</v>
+        <v>15.93818039721589</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -21092,16 +22244,16 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.1486769443332641</v>
+        <v>0.1486769443332642</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2709992587839501</v>
+        <v>0.2709992587839502</v>
       </c>
       <c r="N7" s="8" t="n">
         <v>0.1089293902373044</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.3855864939715396</v>
+        <v>0.3855864939715397</v>
       </c>
       <c r="P7" s="8" t="n">
         <v>11.06225236777087</v>
@@ -21660,19 +22812,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.05284310582563854</v>
+        <v>0.05325271602953684</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>0.1358982294081887</v>
+        <v>0.1370662521804933</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.07000342608673701</v>
+        <v>0.07053630528529894</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>0.229876283738968</v>
+        <v>0.2307655000851229</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>6.059020660904334</v>
+        <v>6.102579719033967</v>
       </c>
     </row>
     <row r="18" ht="42.75" customHeight="1">
@@ -21913,25 +23065,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.2222419530153275</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.305704653263092</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1564661115407944</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.4714254479929222</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>12.27218732237816</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.2167079001665115</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2879326045513153</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.1504430174827576</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.4655189579023732</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>11.64781972765923</v>
+      </c>
     </row>
     <row r="23" ht="57" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -21939,25 +23127,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.06376446783542633</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.2135367393493652</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.08010286837816238</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2525162724170986</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>7.807968556880951</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.06556589156389236</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.2181267142295837</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.08179182559251785</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.2560583753051096</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>7.972198724746704</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -22175,16 +23399,16 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.1934730861495594</v>
+        <v>0.1934730861495593</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.3508298263297102</v>
+        <v>0.3508298263297101</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.1257689352277473</v>
+        <v>0.1257689352277472</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.4398557560718734</v>
+        <v>0.4398557560718733</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>13.53529625332182</v>
@@ -22205,19 +23429,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.1522180623770019</v>
+        <v>0.1522180623770018</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2864085964000331</v>
+        <v>0.286408596400033</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.1002288701696344</v>
+        <v>0.1002288701696343</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.3901513326608047</v>
+        <v>0.3901513326608046</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>10.95373872239176</v>
+        <v>10.95373872239175</v>
       </c>
     </row>
     <row r="8" ht="28.5" customHeight="1">
@@ -22773,19 +23997,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.04334056230404672</v>
+        <v>0.04750289655452618</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>0.1474109581627379</v>
+        <v>0.1457829609537991</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.0587319717531861</v>
+        <v>0.05756569007512276</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>0.2081839626485353</v>
+        <v>0.2179515922275545</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>5.919893669209045</v>
+        <v>5.937173861702152</v>
       </c>
     </row>
     <row r="18" ht="42.75" customHeight="1">
@@ -23026,25 +24250,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.1101136431097984</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2392553091049194</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1003789156675339</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.3318337582431878</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>9.008132666349411</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.09217524528503418</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2124862223863602</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.08952867239713669</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.3036037636213263</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>8.070395141839981</v>
+      </c>
     </row>
     <row r="23" ht="57" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -23052,25 +24312,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.04947250708937645</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1893889456987381</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.07015752047300339</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2224241603094782</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>6.844758242368698</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.05750037729740143</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.2043884992599487</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.07593163847923279</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.2397923628838113</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>7.372330874204636</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -23290,19 +24586,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0001396594965973728</v>
+        <v>0.0001396594965973927</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.009484259124139497</v>
+        <v>0.009484259124140394</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.01317203992458496</v>
+        <v>0.01317203992458562</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.01181776191152</v>
+        <v>0.01181776191152084</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>1.326853884852474</v>
+        <v>1.32685388485254</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -23320,19 +24616,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>9.601332243229078e-05</v>
+        <v>9.601332243228422e-05</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.007809722604800801</v>
+        <v>0.00780972260480095</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.01068584628189106</v>
+        <v>0.01068584628189183</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.009798638805073426</v>
+        <v>0.009798638805073092</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>1.072846166768869</v>
+        <v>1.072846166768947</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -23920,19 +25216,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.07179354717045457</v>
+        <v>0.07178776497778581</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.2294753339016242</v>
+        <v>0.2299949841461413</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.3011921844592256</v>
+        <v>0.3023454230720411</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2679431789959479</v>
+        <v>0.2679323888181229</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>36.80966207554896</v>
+        <v>36.94434214084693</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -23950,19 +25246,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.0679224961821826</v>
+        <v>0.06726067592529583</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.2229321220471367</v>
+        <v>0.2208859765627692</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.2883242366830127</v>
+        <v>0.2849643613343688</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2606194470529446</v>
+        <v>0.2593466327625941</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>35.11959971387677</v>
+        <v>34.70533835623753</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -24141,25 +25437,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.0180140845477581</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1141951978206635</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.1667651832103729</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.1342165583963398</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>16.24061316251755</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.03062155097723007</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1522375345230103</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.2153599858283997</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.1749901453717611</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>21.86572700738907</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -24167,25 +25499,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.02384402416646481</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1409772038459778</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.189256876707077</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1544151034273034</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>18.88814568519592</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.01261968910694122</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.09785348176956177</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.1298185586929321</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1123373896213599</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>12.96799182891846</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -24424,19 +25792,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.004514684671383972</v>
+        <v>0.004514684671383713</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0448830458744384</v>
+        <v>0.04488304587443668</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.08095307078881656</v>
+        <v>0.08095307078881556</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.06719140325505914</v>
+        <v>0.06719140325505721</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>7.624689627706815</v>
+        <v>7.624689627706626</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -24454,19 +25822,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.004233676707906776</v>
+        <v>0.004233676707906693</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.04370332809499343</v>
+        <v>0.04370332809499319</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.07789120348924636</v>
+        <v>0.07789120348924737</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.06506670967481586</v>
+        <v>0.06506670967481522</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>7.369230013605998</v>
+        <v>7.369230013606014</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -25018,23 +26386,23 @@
       </c>
       <c r="K17" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+          <t>{'n_estimators': 200, 'loss': 'square', 'learning_rate': 0.01}</t>
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.06314723507281843</v>
+        <v>0.05810457281080196</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>0.2013782237132013</v>
+        <v>0.1962462277298974</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.3671244578538922</v>
+        <v>0.3726677001002635</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>0.2512911360808782</v>
+        <v>0.2410489012851997</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>33.40782012725396</v>
+        <v>32.22491920875085</v>
       </c>
     </row>
     <row r="18" ht="27.95" customHeight="1">
@@ -25054,19 +26422,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.06780658782231157</v>
+        <v>0.0673205691090504</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.2114211360715016</v>
+        <v>0.2111704635098259</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.3823371647725174</v>
+        <v>0.3806878567737817</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2603969812081384</v>
+        <v>0.2594620764370978</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>35.14016253293456</v>
+        <v>35.09809428201572</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -25084,19 +26452,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.05908927526911058</v>
+        <v>0.05891345947927564</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.1932142970352329</v>
+        <v>0.1922918856237649</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.367170601597429</v>
+        <v>0.370173518602871</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2430828567980691</v>
+        <v>0.2427209498153706</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>31.63620646077019</v>
+        <v>31.4197261038936</v>
       </c>
     </row>
     <row r="19" ht="27.95" customHeight="1">
@@ -25275,25 +26643,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.04595149680972099</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.167851597070694</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.4062642753124237</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2143630024274735</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>27.08903849124908</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.04792823642492294</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1707799583673477</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.421882838010788</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2189251845378301</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>27.37692892551422</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -25301,25 +26705,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.03587181866168976</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.150335282087326</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.2615640759468079</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.1893985709072002</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>21.44909352064133</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.03930814564228058</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.1752880364656448</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.2753732204437256</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1982628196164893</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>24.83091354370117</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -25556,19 +26996,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.002582452554968785</v>
+        <v>0.002582452554968695</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.03592060236116836</v>
+        <v>0.03592060236116754</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.04926472141522924</v>
+        <v>0.04926472141522862</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.05081783697648676</v>
+        <v>0.05081783697648588</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>4.999594455065138</v>
+        <v>4.999594455065064</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -25586,19 +27026,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.002460198617292506</v>
+        <v>0.00246019861729254</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.03601510489323061</v>
+        <v>0.03601510489323051</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.04851128792034148</v>
+        <v>0.04851128792034116</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.04960038928569519</v>
+        <v>0.04960038928569553</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>4.937807798398286</v>
+        <v>4.937807798398258</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -26154,19 +27594,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>0.03572347318165257</v>
+        <v>0.03500913985503729</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>0.1580564254756887</v>
+        <v>0.1563475193109001</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.2543910002551817</v>
+        <v>0.2526334432067287</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>0.189006542695359</v>
+        <v>0.1871072950342591</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>24.30964942241383</v>
+        <v>24.02888121948481</v>
       </c>
     </row>
     <row r="18" ht="56.1" customHeight="1">
@@ -26186,19 +27626,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.062443804853311</v>
+        <v>0.06240747477441169</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.2018604115173273</v>
+        <v>0.201308401689954</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.2851909002249161</v>
+        <v>0.2844864251631732</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2498875844321022</v>
+        <v>0.249814881010743</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>32.47857207951993</v>
+        <v>32.41652994500173</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -26216,19 +27656,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.05129661564611349</v>
+        <v>0.05254619711816116</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.1813825480669757</v>
+        <v>0.1842733201320998</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.2602703127486852</v>
+        <v>0.2644527807279113</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2264875617911798</v>
+        <v>0.2292295729572456</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>28.25767392787322</v>
+        <v>28.79021785737842</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -26407,25 +27847,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.03228428959846497</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.1485264301300049</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.2654401957988739</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.1796782947338519</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>22.64888733625412</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.03166061267256737</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.1461473256349564</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.2611347138881683</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.1779342931325139</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>22.31400907039642</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -26433,25 +27909,61 @@
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.02558156475424767</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.1377114355564117</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.2172682583332062</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.159942379481636</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>19.46834623813629</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Long Short-Term Memory Network</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.01867414638400078</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.117529459297657</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.1835728883743286</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.1366533804338582</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>16.71885401010513</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">

</xml_diff>